<commit_message>
setting up local and remote factory
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\SeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091233D9-65E7-48EA-BE49-5F58B54517D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219BF24F-8B3F-4199-859C-CE1D8EE29AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>titleValidationTest</t>
   </si>
@@ -63,7 +63,10 @@
     <t>expected</t>
   </si>
   <si>
-    <t>(6) Facebook</t>
+    <t>Forgotten Password | Can't Log In | Facebook</t>
+  </si>
+  <si>
+    <t>paymentTest</t>
   </si>
 </sst>
 </file>
@@ -390,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,6 +459,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>